<commit_message>
worked on menu class
</commit_message>
<xml_diff>
--- a/Input Data.xlsx
+++ b/Input Data.xlsx
@@ -25,21 +25,15 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
   <si>
-    <t>Order no.</t>
+    <t>item.no</t>
   </si>
   <si>
-    <t>F_name</t>
+    <t>name</t>
   </si>
   <si>
-    <t>L_name</t>
-  </si>
-  <si>
-    <t>Postcode</t>
-  </si>
-  <si>
-    <t>Phone</t>
+    <t>price</t>
   </si>
 </sst>
 </file>
@@ -357,15 +351,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E21"/>
+  <dimension ref="A1:C29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F1" sqref="F1"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -375,84 +369,78 @@
       <c r="C1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A7">
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A8">
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A9">
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A10">
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A11">
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A12">
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A13">
         <v>12</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A14">
         <v>13</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A15">
         <v>14</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A16">
         <v>15</v>
       </c>
@@ -480,6 +468,46 @@
     <row r="21" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A21">
         <v>20</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A22">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A23">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A24">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A25">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A26">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A27">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="28" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A28">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="29" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A29">
+        <v>28</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Reordered files and made order file, also made excel sheet with menu
</commit_message>
<xml_diff>
--- a/Input Data.xlsx
+++ b/Input Data.xlsx
@@ -12,8 +12,7 @@
     <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7310"/>
   </bookViews>
   <sheets>
-    <sheet name="Orders" sheetId="1" r:id="rId1"/>
-    <sheet name="Customers" sheetId="2" r:id="rId2"/>
+    <sheet name="Menu" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -25,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="47">
   <si>
     <t>item.no</t>
   </si>
@@ -34,6 +33,138 @@
   </si>
   <si>
     <t>price</t>
+  </si>
+  <si>
+    <t>margherita pizza</t>
+  </si>
+  <si>
+    <t>marinara pizza</t>
+  </si>
+  <si>
+    <t>neptuno pizza</t>
+  </si>
+  <si>
+    <t>hawaiian pizza</t>
+  </si>
+  <si>
+    <t>pepperoni pizza</t>
+  </si>
+  <si>
+    <t>funghi pizza</t>
+  </si>
+  <si>
+    <t>tenute bianco 750 ml</t>
+  </si>
+  <si>
+    <t>tenute bianco 175 ml</t>
+  </si>
+  <si>
+    <t>tenute rosso 750 ml</t>
+  </si>
+  <si>
+    <t>tenute rosso 175ml</t>
+  </si>
+  <si>
+    <t>carlindepaolo bianco 750ml</t>
+  </si>
+  <si>
+    <t>carlindepaolo bianco 175ml</t>
+  </si>
+  <si>
+    <t>carlindepaolo rosso 750ml</t>
+  </si>
+  <si>
+    <t>carlindepaolo rosso 175ml</t>
+  </si>
+  <si>
+    <t>francesco bianco 750ml</t>
+  </si>
+  <si>
+    <t>francesco bianco 175ml</t>
+  </si>
+  <si>
+    <t>francesco rosso 750ml</t>
+  </si>
+  <si>
+    <t>francesco rosso 175ml</t>
+  </si>
+  <si>
+    <t>francesco rose 750ml</t>
+  </si>
+  <si>
+    <t>francesco rose 175ml</t>
+  </si>
+  <si>
+    <t>folicello bianco 750ml</t>
+  </si>
+  <si>
+    <t>folicello bianco 175ml</t>
+  </si>
+  <si>
+    <t>folicello rambrusco 750ml</t>
+  </si>
+  <si>
+    <t>folicello rambrusco 175ml</t>
+  </si>
+  <si>
+    <t>lemonade</t>
+  </si>
+  <si>
+    <t>orange juice</t>
+  </si>
+  <si>
+    <t>apple juice</t>
+  </si>
+  <si>
+    <t>sparkling water</t>
+  </si>
+  <si>
+    <t>filtered water</t>
+  </si>
+  <si>
+    <t>mixed salad</t>
+  </si>
+  <si>
+    <t>franco salad</t>
+  </si>
+  <si>
+    <t>oregano</t>
+  </si>
+  <si>
+    <t>garlic</t>
+  </si>
+  <si>
+    <t>olives</t>
+  </si>
+  <si>
+    <t>capers</t>
+  </si>
+  <si>
+    <t>pepperoni</t>
+  </si>
+  <si>
+    <t>anchovies</t>
+  </si>
+  <si>
+    <t>pineapple</t>
+  </si>
+  <si>
+    <t>ham</t>
+  </si>
+  <si>
+    <t>goats cheese</t>
+  </si>
+  <si>
+    <t>mushrooms</t>
+  </si>
+  <si>
+    <t>basil</t>
+  </si>
+  <si>
+    <t>tomato</t>
+  </si>
+  <si>
+    <t>mozzarella</t>
   </si>
 </sst>
 </file>
@@ -351,15 +482,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C29"/>
+  <dimension ref="A1:N32"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" topLeftCell="B3" workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="2" max="2" width="29.08984375" customWidth="1"/>
+    <col min="5" max="5" width="8.7265625" customWidth="1"/>
+    <col min="6" max="6" width="20.08984375" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -369,162 +505,529 @@
       <c r="C1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="L1" t="s">
+        <v>0</v>
+      </c>
+      <c r="M1" t="s">
+        <v>1</v>
+      </c>
+      <c r="N1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="B2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2">
+        <v>4.5</v>
+      </c>
+      <c r="D2" t="s">
+        <v>45</v>
+      </c>
+      <c r="E2" t="s">
+        <v>35</v>
+      </c>
+      <c r="F2" t="s">
+        <v>34</v>
+      </c>
+      <c r="L2">
+        <v>32</v>
+      </c>
+      <c r="M2" t="s">
+        <v>34</v>
+      </c>
+      <c r="N2">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>2</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="B3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C3">
+        <v>5.9</v>
+      </c>
+      <c r="D3" t="s">
+        <v>45</v>
+      </c>
+      <c r="E3" t="s">
+        <v>46</v>
+      </c>
+      <c r="F3" t="s">
+        <v>44</v>
+      </c>
+      <c r="L3">
+        <v>33</v>
+      </c>
+      <c r="M3" t="s">
+        <v>35</v>
+      </c>
+      <c r="N3">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>3</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="B4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4">
+        <v>6.4</v>
+      </c>
+      <c r="D4" t="s">
+        <v>43</v>
+      </c>
+      <c r="E4" t="s">
+        <v>46</v>
+      </c>
+      <c r="F4" t="s">
+        <v>42</v>
+      </c>
+      <c r="G4" t="s">
+        <v>45</v>
+      </c>
+      <c r="L4">
+        <v>34</v>
+      </c>
+      <c r="M4" t="s">
+        <v>36</v>
+      </c>
+      <c r="N4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>4</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="B5" t="s">
+        <v>6</v>
+      </c>
+      <c r="C5">
+        <v>6.85</v>
+      </c>
+      <c r="D5" t="s">
+        <v>41</v>
+      </c>
+      <c r="E5" t="s">
+        <v>46</v>
+      </c>
+      <c r="F5" t="s">
+        <v>40</v>
+      </c>
+      <c r="G5" t="s">
+        <v>45</v>
+      </c>
+      <c r="L5">
+        <v>35</v>
+      </c>
+      <c r="M5" t="s">
+        <v>37</v>
+      </c>
+      <c r="N5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>5</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="B6" t="s">
+        <v>5</v>
+      </c>
+      <c r="C6">
+        <v>6.95</v>
+      </c>
+      <c r="D6" t="s">
+        <v>37</v>
+      </c>
+      <c r="E6" t="s">
+        <v>36</v>
+      </c>
+      <c r="F6" t="s">
+        <v>39</v>
+      </c>
+      <c r="G6" t="s">
+        <v>35</v>
+      </c>
+      <c r="H6" t="s">
+        <v>45</v>
+      </c>
+      <c r="I6" t="s">
+        <v>34</v>
+      </c>
+      <c r="J6" t="s">
+        <v>46</v>
+      </c>
+      <c r="L6">
+        <v>36</v>
+      </c>
+      <c r="M6" t="s">
+        <v>38</v>
+      </c>
+      <c r="N6">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A7">
         <v>6</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="B7" t="s">
+        <v>7</v>
+      </c>
+      <c r="C7">
+        <v>6.85</v>
+      </c>
+      <c r="D7" t="s">
+        <v>45</v>
+      </c>
+      <c r="E7" t="s">
+        <v>46</v>
+      </c>
+      <c r="F7" t="s">
+        <v>38</v>
+      </c>
+      <c r="L7">
+        <v>37</v>
+      </c>
+      <c r="M7" t="s">
+        <v>39</v>
+      </c>
+      <c r="N7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A8">
         <v>7</v>
       </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="B8" t="s">
+        <v>32</v>
+      </c>
+      <c r="C8">
+        <v>2.4500000000000002</v>
+      </c>
+      <c r="L8">
+        <v>38</v>
+      </c>
+      <c r="M8" t="s">
+        <v>40</v>
+      </c>
+      <c r="N8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A9">
         <v>8</v>
       </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="B9" t="s">
+        <v>33</v>
+      </c>
+      <c r="C9">
+        <v>3.55</v>
+      </c>
+      <c r="L9">
+        <v>39</v>
+      </c>
+      <c r="M9" t="s">
+        <v>41</v>
+      </c>
+      <c r="N9">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A10">
         <v>9</v>
       </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="B10" t="s">
+        <v>9</v>
+      </c>
+      <c r="C10">
+        <v>14.95</v>
+      </c>
+      <c r="L10">
+        <v>40</v>
+      </c>
+      <c r="M10" t="s">
+        <v>42</v>
+      </c>
+      <c r="N10">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A11">
         <v>10</v>
       </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="B11" t="s">
+        <v>10</v>
+      </c>
+      <c r="C11">
+        <v>3.9</v>
+      </c>
+      <c r="L11">
+        <v>41</v>
+      </c>
+      <c r="M11" t="s">
+        <v>43</v>
+      </c>
+      <c r="N11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A12">
         <v>11</v>
       </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="B12" t="s">
+        <v>11</v>
+      </c>
+      <c r="C12">
+        <v>14.95</v>
+      </c>
+      <c r="L12">
+        <v>42</v>
+      </c>
+      <c r="M12" t="s">
+        <v>44</v>
+      </c>
+      <c r="N12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A13">
         <v>12</v>
       </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="B13" t="s">
+        <v>12</v>
+      </c>
+      <c r="C13">
+        <v>3.9</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A14">
         <v>13</v>
       </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="B14" t="s">
+        <v>13</v>
+      </c>
+      <c r="C14">
+        <v>15.95</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A15">
         <v>14</v>
       </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="B15" t="s">
+        <v>14</v>
+      </c>
+      <c r="C15">
+        <v>4.1500000000000004</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A16">
         <v>15</v>
       </c>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B16" t="s">
+        <v>15</v>
+      </c>
+      <c r="C16">
+        <v>15.95</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A17">
         <v>16</v>
       </c>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B17" t="s">
+        <v>16</v>
+      </c>
+      <c r="C17">
+        <v>4.1500000000000004</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A18">
         <v>17</v>
       </c>
-    </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B18" t="s">
+        <v>17</v>
+      </c>
+      <c r="C18">
+        <v>17.95</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A19">
         <v>18</v>
       </c>
-    </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B19" t="s">
+        <v>18</v>
+      </c>
+      <c r="C19">
+        <v>4.5</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A20">
         <v>19</v>
       </c>
-    </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B20" t="s">
+        <v>19</v>
+      </c>
+      <c r="C20">
+        <v>17.95</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A21">
         <v>20</v>
       </c>
-    </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B21" t="s">
+        <v>20</v>
+      </c>
+      <c r="C21">
+        <v>4.5</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A22">
         <v>21</v>
       </c>
-    </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B22" t="s">
+        <v>21</v>
+      </c>
+      <c r="C22">
+        <v>17.95</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A23">
         <v>22</v>
       </c>
-    </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B23" t="s">
+        <v>22</v>
+      </c>
+      <c r="C23">
+        <v>4.5</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A24">
         <v>23</v>
       </c>
-    </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B24" t="s">
+        <v>23</v>
+      </c>
+      <c r="C24">
+        <v>19.5</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A25">
         <v>24</v>
       </c>
-    </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B25" t="s">
+        <v>24</v>
+      </c>
+      <c r="C25">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A26">
         <v>25</v>
       </c>
-    </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B26" t="s">
+        <v>25</v>
+      </c>
+      <c r="C26">
+        <v>19.5</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A27">
         <v>26</v>
       </c>
-    </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B27" t="s">
+        <v>26</v>
+      </c>
+      <c r="C27">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A28">
         <v>27</v>
       </c>
-    </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B28" t="s">
+        <v>27</v>
+      </c>
+      <c r="C28">
+        <v>2.2000000000000002</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A29">
         <v>28</v>
+      </c>
+      <c r="B29" t="s">
+        <v>28</v>
+      </c>
+      <c r="C29">
+        <v>2.5499999999999998</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A30">
+        <v>29</v>
+      </c>
+      <c r="B30" t="s">
+        <v>29</v>
+      </c>
+      <c r="C30">
+        <v>2.5499999999999998</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A31">
+        <v>30</v>
+      </c>
+      <c r="B31" t="s">
+        <v>30</v>
+      </c>
+      <c r="C31">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A32">
+        <v>31</v>
+      </c>
+      <c r="B32" t="s">
+        <v>31</v>
+      </c>
+      <c r="C32">
+        <v>0</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D16" sqref="D16:D17"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>